<commit_message>
feat: out excel add some properties
</commit_message>
<xml_diff>
--- a/storage/src/main/resources/excel/outStorage.xlsx
+++ b/storage/src/main/resources/excel/outStorage.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>订单明细</t>
   </si>
@@ -56,9 +56,15 @@
     <t>入库数量</t>
   </si>
   <si>
+    <t>出库类型</t>
+  </si>
+  <si>
     <t>出库数量</t>
   </si>
   <si>
+    <t>剩余数量</t>
+  </si>
+  <si>
     <t>{.code}</t>
   </si>
   <si>
@@ -83,7 +89,13 @@
     <t>{.inCount}</t>
   </si>
   <si>
+    <t>{.outType}</t>
+  </si>
+  <si>
     <t>{.bunchCount}</t>
+  </si>
+  <si>
+    <t>{.leftPartSumCount}</t>
   </si>
 </sst>
 </file>
@@ -459,7 +471,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -471,6 +483,43 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -606,7 +655,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -618,34 +667,34 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -730,7 +779,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -746,23 +795,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1083,144 +1138,163 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="13.5" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="5" width="40.625" style="3" customWidth="1"/>
     <col min="6" max="8" width="30.625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="20.625" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="8.725" style="3"/>
+    <col min="9" max="11" width="20.625" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="8.725" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="40" customHeight="1" spans="1:9">
+    <row r="1" s="1" customFormat="1" ht="40" customHeight="1" spans="1:11">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="12"/>
     </row>
-    <row r="2" s="2" customFormat="1" ht="21" customHeight="1" spans="1:9">
-      <c r="A2" s="5" t="s">
+    <row r="2" s="2" customFormat="1" ht="21" customHeight="1" spans="1:11">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="J2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="23" customHeight="1" spans="1:9">
-      <c r="A3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="9" t="s">
+    <row r="3" s="1" customFormat="1" ht="23" customHeight="1" spans="1:11">
+      <c r="A3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="C3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="F3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="G3" s="9" t="s">
         <v>18</v>
       </c>
+      <c r="H3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="3:10">
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
+    <row r="4" spans="3:11">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
     </row>
-    <row r="5" spans="3:10">
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
+    <row r="5" spans="3:11">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
     </row>
-    <row r="6" spans="3:10">
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+    <row r="6" spans="3:11">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
     </row>
-    <row r="7" spans="3:10">
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
+    <row r="7" spans="3:11">
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
     </row>
-    <row r="8" spans="3:10">
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+    <row r="8" spans="3:11">
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>